<commit_message>
update on dataclass and porting
updated validators
updated 5 split from SeroNet to ImmPort
</commit_message>
<xml_diff>
--- a/seronetTemplates/SeroNet Registry Template 0.99 mapping to ImmPort mar 2.xlsx
+++ b/seronetTemplates/SeroNet Registry Template 0.99 mapping to ImmPort mar 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\freundelt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liualg/Documents/GitHub/SeroNet/seronetTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BBAA4A0-2073-4517-A07F-85F02109DA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35EC410-75F1-9F4C-B1C4-104F3E08E9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29145" yWindow="510" windowWidth="25110" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20580" yWindow="500" windowWidth="15260" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="basic_study_design.txt" sheetId="1" r:id="rId1"/>
@@ -58,43 +58,15 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>The identifier should be unique to the ImmPort workspace to which the data will be uploaded.  The template column is associated with the following database table column study.user_defined_id and has data type varchar(150)</t>
         </r>
       </text>
     </comment>
     <comment ref="D6" authorId="1" shapeId="0" xr:uid="{99F36443-8FFF-4E37-A7EC-505AD407144F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>An identifier that is unique to SeroNet and ImmPort. PMIDXXXXXX_study</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The brief title serves as a working title for a study.  The template column is associated with the following database table column study.brief_title and has data type varchar(250)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{2A44B118-9DA3-4E8E-807C-415DD93AEB70}">
       <text>
         <r>
           <rPr>
@@ -103,25 +75,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Brief yet descriptive title of the study.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The official study title may be the same as the brief title, but is often more descriptive.  The template column is associated with the following database table column study.official_title and has data type varchar(500)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="1" shapeId="0" xr:uid="{87B554C8-423D-4D40-A86B-17BFACBEF5F8}">
+          <t>An identifier that is unique to SeroNet and ImmPort. PMIDXXXXXX_study</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>The brief title serves as a working title for a study.  The template column is associated with the following database table column study.brief_title and has data type varchar(250)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{2A44B118-9DA3-4E8E-807C-415DD93AEB70}">
       <text>
         <r>
           <rPr>
@@ -130,25 +101,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The official title of the manuscript generated by the study.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Summarize the goals, methods and results of the study.  The template column is associated with the following database table column study.brief_description and has data type varchar(4000)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D9" authorId="1" shapeId="0" xr:uid="{9F013221-48F7-4309-BAC1-AE74EB26A89D}">
+          <t>Brief yet descriptive title of the study.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The official study title may be the same as the brief title, but is often more descriptive.  The template column is associated with the following database table column study.official_title and has data type varchar(500)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="1" shapeId="0" xr:uid="{87B554C8-423D-4D40-A86B-17BFACBEF5F8}">
       <text>
         <r>
           <rPr>
@@ -157,11 +128,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Short narrative describing the principle objectives of the study.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F9" authorId="1" shapeId="0" xr:uid="{27F54E1D-98DE-4D52-84BB-C23B20414777}">
+          <t>The official title of the manuscript generated by the study.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Summarize the goals, methods and results of the study.  The template column is associated with the following database table column study.brief_description and has data type varchar(4000)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="1" shapeId="0" xr:uid="{9F013221-48F7-4309-BAC1-AE74EB26A89D}">
       <text>
         <r>
           <rPr>
@@ -170,25 +154,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">A coded value that represents the plan of how a study will be performed in order to represent the phenomenon under examination, to answer the research questions that have been asked, and defining the methods of data analysis. Select from drop down. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The detailed description supports a lengthy description of the goals and methods of the study.  The template column is associated with the following database table column study.description and has data type clob</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D10" authorId="1" shapeId="0" xr:uid="{D1CED6F9-AC37-4951-8044-6A5C0A72A679}">
+          <t>Short narrative describing the principle objectives of the study.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="1" shapeId="0" xr:uid="{27F54E1D-98DE-4D52-84BB-C23B20414777}">
       <text>
         <r>
           <rPr>
@@ -197,11 +167,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Excerpt of abstract which includes information about data collected. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F10" authorId="1" shapeId="0" xr:uid="{64B5CD3E-F59F-41FF-82CC-98D7F4271ABF}">
+          <t xml:space="preserve">A coded value that represents the plan of how a study will be performed in order to represent the phenomenon under examination, to answer the research questions that have been asked, and defining the methods of data analysis. Select from drop down. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The detailed description supports a lengthy description of the goals and methods of the study.  The template column is associated with the following database table column study.description and has data type clob</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="1" shapeId="0" xr:uid="{D1CED6F9-AC37-4951-8044-6A5C0A72A679}">
       <text>
         <r>
           <rPr>
@@ -210,25 +194,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The type(s) of in silico models that were developed as part of the study. Select from drop down</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>IA brief description of the study's interventional component (e.g. influenza vaccine).  The template column is associated with the following database table column study.intervention_agent and has data type varchar(1000)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="1" shapeId="0" xr:uid="{9D1051A5-4D37-405A-A36B-DD524C96F2EC}">
+          <t xml:space="preserve">Excerpt of abstract which includes information about data collected. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="1" shapeId="0" xr:uid="{64B5CD3E-F59F-41FF-82CC-98D7F4271ABF}">
       <text>
         <r>
           <rPr>
@@ -237,39 +207,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The SARS-CoV-2 vaccine administered to study subjects included in the study. Select from drop down.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Endpoints include assessments, lab tests and assays that are part of a study design.  The template column is associated with the following database table column study.endpoints and has data type clob</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The organization that provides funding and support for the study.  The template column is associated with the following database table column study.sponsoring_organization and has data type varchar(250)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D13" authorId="1" shapeId="0" xr:uid="{3B56FC69-E2AB-4F1B-B0BC-39A2C63671BD}">
+          <t>The type(s) of in silico models that were developed as part of the study. Select from drop down</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>IA brief description of the study's interventional component (e.g. influenza vaccine).  The template column is associated with the following database table column study.intervention_agent and has data type varchar(1000)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="1" shapeId="0" xr:uid="{9D1051A5-4D37-405A-A36B-DD524C96F2EC}">
       <text>
         <r>
           <rPr>
@@ -278,25 +234,39 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Full official name of the institution or organization at which the study was conducted.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The unit of time used to describe the subject's age in the study.  The unit of time for a subject must conform to this unit.  The template column is associated with the following database table column study.age_unit and has data type varchar(25)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D14" authorId="1" shapeId="0" xr:uid="{959C3BFB-58D6-4E43-873B-4FB045BB96BE}">
+          <t>The SARS-CoV-2 vaccine administered to study subjects included in the study. Select from drop down.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Endpoints include assessments, lab tests and assays that are part of a study design.  The template column is associated with the following database table column study.endpoints and has data type clob</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The organization that provides funding and support for the study.  The template column is associated with the following database table column study.sponsoring_organization and has data type varchar(250)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="1" shapeId="0" xr:uid="{3B56FC69-E2AB-4F1B-B0BC-39A2C63671BD}">
       <text>
         <r>
           <rPr>
@@ -305,25 +275,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The unit of time used to describe the subject's age in the study; must conform Year.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The commencement time point of the study. The date format is either dd-MMM-yy or dd-MMM-yyyy.   The template column is associated with the following database table column study.actual_start_date and has data type date</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D15" authorId="1" shapeId="0" xr:uid="{5E770E9B-38D6-4924-A6FD-5E5E0D0EEDC8}">
+          <t>Full official name of the institution or organization at which the study was conducted.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The unit of time used to describe the subject's age in the study.  The unit of time for a subject must conform to this unit.  The template column is associated with the following database table column study.age_unit and has data type varchar(25)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D14" authorId="1" shapeId="0" xr:uid="{959C3BFB-58D6-4E43-873B-4FB045BB96BE}">
       <text>
         <r>
           <rPr>
@@ -332,53 +302,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Date upon which the first study subject was enrolled into the study. The date format is dd-MM-yyyy. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The explanatory proposition(s) being tested by the research study.  The template column is associated with the following database table column study.hypothesis and has data type varchar(4000)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The goals of the research study.  The template column is associated with the following database table column study.objectives and has data type clob</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The number of subjects proposed to be enrolled in the study.  The template column is associated with the following database table column study.target_enrollment and has data type integer</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D18" authorId="1" shapeId="0" xr:uid="{F9F2290D-939B-4FCB-A290-57FA0D493FB7}">
+          <t>The unit of time used to describe the subject's age in the study; must conform Year.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The commencement time point of the study. The date format is either dd-MMM-yy or dd-MMM-yyyy.   The template column is associated with the following database table column study.actual_start_date and has data type date</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="1" shapeId="0" xr:uid="{5E770E9B-38D6-4924-A6FD-5E5E0D0EEDC8}">
       <text>
         <r>
           <rPr>
@@ -387,25 +329,53 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The total number of study subjects included in the study.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The minimum age of subjects enrolled in the study.  The template column is associated with the following database table column study.minimum_age and has data type varchar(40)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D19" authorId="1" shapeId="0" xr:uid="{0F271CC3-E759-416C-B38B-3FA09B556AA4}">
+          <t xml:space="preserve">Date upon which the first study subject was enrolled into the study. The date format is dd-MM-yyyy. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The explanatory proposition(s) being tested by the research study.  The template column is associated with the following database table column study.hypothesis and has data type varchar(4000)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The goals of the research study.  The template column is associated with the following database table column study.objectives and has data type clob</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The number of subjects proposed to be enrolled in the study.  The template column is associated with the following database table column study.target_enrollment and has data type integer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="1" shapeId="0" xr:uid="{F9F2290D-939B-4FCB-A290-57FA0D493FB7}">
       <text>
         <r>
           <rPr>
@@ -414,25 +384,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The ages of the subjects recruited for the study expressed as a range.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>The maximum age of subjects enrolled in the study.  The template column is associated with the following database table column study.maximum_age and has data type varchar(40)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D20" authorId="1" shapeId="0" xr:uid="{EE536881-8B39-41AD-B874-DCE2A5ED3B1B}">
+          <t>The total number of study subjects included in the study.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>The minimum age of subjects enrolled in the study.  The template column is associated with the following database table column study.minimum_age and has data type varchar(40)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="1" shapeId="0" xr:uid="{0F271CC3-E759-416C-B38B-3FA09B556AA4}">
       <text>
         <r>
           <rPr>
@@ -445,15 +415,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>The maximum age of subjects enrolled in the study.  The template column is associated with the following database table column study.maximum_age and has data type varchar(40)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D20" authorId="1" shapeId="0" xr:uid="{EE536881-8B39-41AD-B874-DCE2A5ED3B1B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The ages of the subjects recruited for the study expressed as a range.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
             <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Please use the drop down list  The template column is associated with the following database table column study_categorization.research_focus and has data type varchar(50)</t>
         </r>
@@ -5433,12 +5428,14 @@
       <sz val="9"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -5912,6 +5909,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5923,24 +5938,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6661,34 +6658,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" customWidth="1"/>
-    <col min="5" max="12" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="40.5" customWidth="1"/>
+    <col min="5" max="12" width="25.5" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="18.109375" customWidth="1"/>
-    <col min="23" max="23" width="23.21875" customWidth="1"/>
-    <col min="24" max="24" width="14.5546875" customWidth="1"/>
-    <col min="25" max="25" width="23.5546875" customWidth="1"/>
-    <col min="27" max="28" width="18.77734375" customWidth="1"/>
-    <col min="29" max="29" width="19.44140625" customWidth="1"/>
+    <col min="15" max="15" width="18.1640625" customWidth="1"/>
+    <col min="23" max="23" width="23.1640625" customWidth="1"/>
+    <col min="24" max="24" width="14.5" customWidth="1"/>
+    <col min="25" max="25" width="23.5" customWidth="1"/>
+    <col min="27" max="28" width="18.83203125" customWidth="1"/>
+    <col min="29" max="29" width="19.5" customWidth="1"/>
     <col min="30" max="30" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="27" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6696,13 +6693,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="78" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="75" t="s">
         <v>513</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -6710,8 +6707,8 @@
       </c>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="78"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="75"/>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -6720,8 +6717,8 @@
         <v>463</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="78"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="75"/>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -6733,8 +6730,8 @@
         <v>478</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="78"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="75"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
@@ -6746,8 +6743,8 @@
         <v>475</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="78"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="75"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
@@ -6759,8 +6756,8 @@
         <v>476</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="78"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="75"/>
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
@@ -6772,8 +6769,8 @@
         <v>477</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="78"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="75"/>
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
@@ -6785,8 +6782,8 @@
         <v>691</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="78"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="75"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -6794,10 +6791,10 @@
       <c r="D12" s="12" t="s">
         <v>690</v>
       </c>
-      <c r="E12" s="81"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="78"/>
+      <c r="E12" s="73"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="75"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
@@ -6806,8 +6803,8 @@
         <v>467</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="78"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="75"/>
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
@@ -6816,8 +6813,8 @@
         <v>469</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="78"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="75"/>
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
@@ -6826,8 +6823,8 @@
         <v>470</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="78"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="75"/>
       <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
@@ -6836,8 +6833,8 @@
         <v>479</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="78"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="75"/>
       <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
@@ -6846,8 +6843,8 @@
         <v>490</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="78"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="75"/>
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
@@ -6856,8 +6853,8 @@
         <v>471</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="78"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="75"/>
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
@@ -6866,8 +6863,8 @@
         <v>472</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="78"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="75"/>
       <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
@@ -6876,11 +6873,11 @@
         <v>473</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="78"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="78"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="75"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="75"/>
       <c r="B22" s="5" t="s">
         <v>29</v>
       </c>
@@ -6889,8 +6886,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="78"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="75"/>
       <c r="B23" s="3" t="s">
         <v>30</v>
       </c>
@@ -6899,11 +6896,11 @@
         <v>658</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="78"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="78"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="75"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="75"/>
       <c r="B25" s="5" t="s">
         <v>46</v>
       </c>
@@ -6912,8 +6909,8 @@
         <v>474</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A26" s="78"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="75"/>
       <c r="B26" s="3" t="s">
         <v>47</v>
       </c>
@@ -6925,11 +6922,11 @@
         <v>649</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="78"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="78"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="75"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="75"/>
       <c r="B28" s="5" t="s">
         <v>389</v>
       </c>
@@ -6937,8 +6934,8 @@
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="78"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="75"/>
       <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
@@ -6952,8 +6949,8 @@
         <v>391</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="78"/>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="75"/>
       <c r="B30" s="15" t="s">
         <v>609</v>
       </c>
@@ -6967,8 +6964,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="78"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="75"/>
       <c r="B31" s="7" t="s">
         <v>590</v>
       </c>
@@ -6982,11 +6979,11 @@
         <v>601</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="78"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="78"/>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="75"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="75"/>
       <c r="B33" s="5" t="s">
         <v>405</v>
       </c>
@@ -7001,8 +6998,8 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="78"/>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="75"/>
       <c r="B34" s="3" t="s">
         <v>610</v>
       </c>
@@ -7037,8 +7034,8 @@
         <v>415</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="24" x14ac:dyDescent="0.3">
-      <c r="A35" s="78"/>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="75"/>
       <c r="B35" s="7" t="s">
         <v>659</v>
       </c>
@@ -7073,11 +7070,11 @@
         <v>489</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="78"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="78"/>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="75"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="75"/>
       <c r="B37" s="5" t="s">
         <v>421</v>
       </c>
@@ -7088,8 +7085,8 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="78"/>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="75"/>
       <c r="B38" s="3" t="s">
         <v>5</v>
       </c>
@@ -7112,8 +7109,8 @@
         <v>426</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="24" x14ac:dyDescent="0.3">
-      <c r="A39" s="78"/>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="75"/>
       <c r="B39" s="62" t="s">
         <v>602</v>
       </c>
@@ -7136,19 +7133,19 @@
         <v>608</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="78"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="78"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="75"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="75"/>
       <c r="B41" s="5" t="s">
         <v>427</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="78"/>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="75"/>
       <c r="B42" s="3" t="s">
         <v>5</v>
       </c>
@@ -7159,8 +7156,8 @@
         <v>429</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="24" x14ac:dyDescent="0.3">
-      <c r="A43" s="78"/>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="75"/>
       <c r="B43" s="62" t="s">
         <v>611</v>
       </c>
@@ -7171,40 +7168,40 @@
         <v>613</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="78"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="78"/>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="75"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="75"/>
       <c r="B45" s="5" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="78"/>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="75"/>
       <c r="B46" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="78"/>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="75"/>
       <c r="B47" s="62" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="78"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A49" s="78"/>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="75"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="75"/>
       <c r="B49" s="5" t="s">
         <v>433</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A50" s="78"/>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" s="75"/>
       <c r="B50" s="3" t="s">
         <v>434</v>
       </c>
@@ -7215,8 +7212,8 @@
         <v>435</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="24" x14ac:dyDescent="0.3">
-      <c r="A51" s="78"/>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" s="75"/>
       <c r="B51" s="62" t="s">
         <v>616</v>
       </c>
@@ -7227,18 +7224,18 @@
         <v>618</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A52" s="78"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A53" s="78"/>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" s="75"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" s="75"/>
       <c r="B53" s="5" t="s">
         <v>451</v>
       </c>
       <c r="C53" s="5"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A54" s="78"/>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" s="75"/>
       <c r="B54" s="3" t="s">
         <v>390</v>
       </c>
@@ -7246,8 +7243,8 @@
         <v>452</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A55" s="78"/>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="75"/>
       <c r="B55" s="62" t="s">
         <v>619</v>
       </c>
@@ -7256,11 +7253,11 @@
       </c>
       <c r="D55" s="25"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A56" s="78"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A57" s="78"/>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" s="75"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" s="75"/>
       <c r="B57" s="18" t="s">
         <v>453</v>
       </c>
@@ -7273,8 +7270,8 @@
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A58" s="78"/>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" s="75"/>
       <c r="B58" s="3" t="s">
         <v>454</v>
       </c>
@@ -7303,13 +7300,13 @@
         <v>462</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A59" s="78"/>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" s="75"/>
       <c r="B59" s="10" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="N61" s="13" t="s">
         <v>642</v>
       </c>
@@ -7317,8 +7314,8 @@
         <v>642</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A62" s="76" t="s">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" s="77" t="s">
         <v>521</v>
       </c>
       <c r="B62" s="22" t="s">
@@ -7333,13 +7330,13 @@
       <c r="I62" s="23"/>
       <c r="J62" s="23"/>
       <c r="K62" s="23"/>
-      <c r="L62" s="77"/>
-      <c r="M62" s="77"/>
-      <c r="N62" s="77"/>
-      <c r="O62" s="77"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A63" s="76"/>
+      <c r="L62" s="74"/>
+      <c r="M62" s="74"/>
+      <c r="N62" s="74"/>
+      <c r="O62" s="74"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" s="77"/>
       <c r="B63" s="17" t="s">
         <v>492</v>
       </c>
@@ -7383,8 +7380,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="76"/>
+    <row r="64" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="77"/>
       <c r="B64" s="26" t="s">
         <v>509</v>
       </c>
@@ -7426,8 +7423,8 @@
         <v>641</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="76"/>
+    <row r="65" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="77"/>
       <c r="B65" s="20" t="s">
         <v>492</v>
       </c>
@@ -7468,8 +7465,8 @@
         <v>501</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="76"/>
+    <row r="66" spans="1:25" ht="42.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="77"/>
       <c r="B66" s="26" t="s">
         <v>592</v>
       </c>
@@ -7508,23 +7505,23 @@
         <v>631</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A67" s="76"/>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A68" s="76"/>
-      <c r="B68" s="79" t="s">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A67" s="77"/>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A68" s="77"/>
+      <c r="B68" s="76" t="s">
         <v>520</v>
       </c>
-      <c r="C68" s="77"/>
-      <c r="D68" s="77"/>
-      <c r="E68" s="77"/>
-      <c r="F68" s="77"/>
-      <c r="G68" s="77"/>
-      <c r="H68" s="77"/>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A69" s="76"/>
+      <c r="C68" s="74"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
+      <c r="F68" s="74"/>
+      <c r="G68" s="74"/>
+      <c r="H68" s="74"/>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A69" s="77"/>
       <c r="B69" s="17" t="s">
         <v>492</v>
       </c>
@@ -7548,8 +7545,8 @@
       </c>
       <c r="I69" s="48"/>
     </row>
-    <row r="70" spans="1:25" ht="34.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A70" s="76"/>
+    <row r="70" spans="1:25" ht="39" x14ac:dyDescent="0.2">
+      <c r="A70" s="77"/>
       <c r="B70" s="26" t="s">
         <v>509</v>
       </c>
@@ -7570,8 +7567,8 @@
         <v>526</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="34.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A71" s="76"/>
+    <row r="71" spans="1:25" ht="39" x14ac:dyDescent="0.2">
+      <c r="A71" s="77"/>
       <c r="B71" s="27" t="s">
         <v>592</v>
       </c>
@@ -7592,7 +7589,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D72" s="13" t="s">
         <v>692</v>
       </c>
@@ -7600,9 +7597,9 @@
         <v>527</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="77" spans="1:25" ht="48.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="76" t="s">
+    <row r="76" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:25" ht="48.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="77" t="s">
         <v>559</v>
       </c>
       <c r="B77" s="20" t="s">
@@ -7678,8 +7675,8 @@
         <v>558</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A78" s="76"/>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A78" s="77"/>
       <c r="B78" s="55" t="s">
         <v>4</v>
       </c>
@@ -7699,8 +7696,8 @@
         <v>528</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="76"/>
+    <row r="79" spans="1:25" ht="35.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="77"/>
       <c r="B79" s="26" t="s">
         <v>509</v>
       </c>
@@ -7732,8 +7729,8 @@
         <v>676</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="34.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A80" s="76"/>
+    <row r="80" spans="1:25" ht="26" x14ac:dyDescent="0.2">
+      <c r="A80" s="77"/>
       <c r="B80" s="27" t="s">
         <v>592</v>
       </c>
@@ -7747,8 +7744,8 @@
       <c r="F80" s="29"/>
       <c r="G80" s="29"/>
     </row>
-    <row r="81" spans="1:16" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A81" s="76"/>
+    <row r="81" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+      <c r="A81" s="77"/>
       <c r="C81" s="28" t="s">
         <v>529</v>
       </c>
@@ -7759,8 +7756,8 @@
       <c r="F81" s="29"/>
       <c r="G81" s="29"/>
     </row>
-    <row r="82" spans="1:16" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="76"/>
+    <row r="82" spans="1:16" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="77"/>
       <c r="C82" s="28" t="s">
         <v>529</v>
       </c>
@@ -7771,12 +7768,12 @@
       <c r="F82" s="29"/>
       <c r="G82" s="29"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E83" s="13" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="84" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H84"/>
       <c r="I84"/>
       <c r="J84"/>
@@ -7787,8 +7784,8 @@
       <c r="O84"/>
       <c r="P84"/>
     </row>
-    <row r="85" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="76" t="s">
+    <row r="85" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="77" t="s">
         <v>562</v>
       </c>
       <c r="B85" s="53" t="s">
@@ -7796,8 +7793,8 @@
       </c>
       <c r="G85" s="30"/>
     </row>
-    <row r="86" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="76"/>
+    <row r="86" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="77"/>
       <c r="B86" s="42" t="s">
         <v>5</v>
       </c>
@@ -7817,8 +7814,8 @@
         <v>561</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A87" s="76"/>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A87" s="77"/>
       <c r="B87" s="9" t="s">
         <v>530</v>
       </c>
@@ -7838,8 +7835,8 @@
         <v>673</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A88" s="76"/>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A88" s="77"/>
       <c r="B88" s="7" t="s">
         <v>662</v>
       </c>
@@ -7859,12 +7856,12 @@
         <v>498</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D89" s="13" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="B90" s="31"/>
       <c r="C90" s="30"/>
       <c r="D90" s="30"/>
@@ -7874,7 +7871,7 @@
       <c r="H90" s="33"/>
       <c r="I90" s="33"/>
     </row>
-    <row r="91" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="B91" s="31"/>
       <c r="C91" s="30"/>
       <c r="D91" s="30"/>
@@ -7884,8 +7881,8 @@
       <c r="H91" s="33"/>
       <c r="I91" s="33"/>
     </row>
-    <row r="93" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="75" t="s">
+    <row r="93" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="81" t="s">
         <v>594</v>
       </c>
       <c r="B93" s="53" t="s">
@@ -7899,8 +7896,8 @@
       <c r="H93" s="54"/>
       <c r="I93" s="54"/>
     </row>
-    <row r="94" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="75"/>
+    <row r="94" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="81"/>
       <c r="B94" s="40" t="s">
         <v>5</v>
       </c>
@@ -7929,8 +7926,8 @@
         <v>645</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A95" s="75"/>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A95" s="81"/>
       <c r="B95" s="9" t="s">
         <v>536</v>
       </c>
@@ -7939,8 +7936,8 @@
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
     </row>
-    <row r="96" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="75"/>
+    <row r="96" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="81"/>
       <c r="B96" s="7" t="s">
         <v>660</v>
       </c>
@@ -7958,7 +7955,7 @@
       </c>
       <c r="G96" s="34"/>
     </row>
-    <row r="97" spans="1:30" s="48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:30" s="48" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="45"/>
       <c r="B97" s="46"/>
       <c r="C97" s="47"/>
@@ -7966,7 +7963,7 @@
       <c r="E97" s="47"/>
       <c r="G97" s="49"/>
     </row>
-    <row r="98" spans="1:30" s="48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:30" s="48" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="45"/>
       <c r="B98" s="46"/>
       <c r="C98" s="47"/>
@@ -7974,7 +7971,7 @@
       <c r="E98" s="47"/>
       <c r="G98" s="49"/>
     </row>
-    <row r="99" spans="1:30" s="48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:30" s="48" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="45"/>
       <c r="B99" s="46"/>
       <c r="C99" s="47"/>
@@ -7982,7 +7979,7 @@
       <c r="E99" s="47"/>
       <c r="G99" s="49"/>
     </row>
-    <row r="100" spans="1:30" s="48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:30" s="48" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="45"/>
       <c r="B100" s="46"/>
       <c r="C100" s="47"/>
@@ -7990,7 +7987,7 @@
       <c r="E100" s="47"/>
       <c r="G100" s="49"/>
     </row>
-    <row r="101" spans="1:30" s="48" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:30" s="48" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="45"/>
       <c r="B101" s="46"/>
       <c r="C101" s="47"/>
@@ -7998,7 +7995,7 @@
       <c r="E101" s="47"/>
       <c r="G101" s="49"/>
     </row>
-    <row r="102" spans="1:30" s="48" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:30" s="48" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="45"/>
       <c r="B102" s="53" t="s">
         <v>588</v>
@@ -8011,7 +8008,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="103" spans="1:30" s="48" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:30" s="48" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="45"/>
       <c r="B103" s="2" t="s">
         <v>5</v>
@@ -8053,7 +8050,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="104" spans="1:30" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:30" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="45"/>
       <c r="B104" s="55" t="s">
         <v>647</v>
@@ -8079,7 +8076,7 @@
       <c r="M104" s="55"/>
       <c r="N104" s="57"/>
     </row>
-    <row r="105" spans="1:30" s="48" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:30" s="48" customFormat="1" ht="26" x14ac:dyDescent="0.2">
       <c r="A105" s="45"/>
       <c r="B105" s="7" t="s">
         <v>661</v>
@@ -8111,19 +8108,19 @@
       </c>
       <c r="N105" s="57"/>
     </row>
-    <row r="106" spans="1:30" s="56" customFormat="1" ht="12" x14ac:dyDescent="0.3">
-      <c r="C106" s="80" t="s">
+    <row r="106" spans="1:30" s="56" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="C106" s="72" t="s">
         <v>687</v>
       </c>
       <c r="G106" s="27" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="107" spans="1:30" s="56" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="1:30" s="56" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="1:30" s="56" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="110" spans="1:30" s="56" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="111" spans="1:30" s="48" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:30" s="56" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="108" spans="1:30" s="56" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="109" spans="1:30" s="56" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="110" spans="1:30" s="56" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="111" spans="1:30" s="48" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="45"/>
       <c r="B111" s="46"/>
       <c r="C111" s="47"/>
@@ -8131,7 +8128,7 @@
       <c r="E111" s="47"/>
       <c r="G111" s="49"/>
     </row>
-    <row r="112" spans="1:30" s="48" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:30" s="48" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="45"/>
       <c r="B112" s="46" t="s">
         <v>646</v>
@@ -8140,29 +8137,29 @@
       <c r="D112" s="47"/>
       <c r="E112" s="47"/>
       <c r="G112" s="49"/>
-      <c r="O112" s="72" t="s">
+      <c r="O112" s="78" t="s">
         <v>679</v>
       </c>
-      <c r="P112" s="73"/>
-      <c r="Q112" s="73"/>
-      <c r="R112" s="73"/>
-      <c r="S112" s="73"/>
-      <c r="T112" s="73"/>
-      <c r="U112" s="73"/>
-      <c r="V112" s="74"/>
-      <c r="W112" s="72" t="s">
+      <c r="P112" s="79"/>
+      <c r="Q112" s="79"/>
+      <c r="R112" s="79"/>
+      <c r="S112" s="79"/>
+      <c r="T112" s="79"/>
+      <c r="U112" s="79"/>
+      <c r="V112" s="80"/>
+      <c r="W112" s="78" t="s">
         <v>680</v>
       </c>
-      <c r="X112" s="73"/>
-      <c r="Y112" s="73"/>
-      <c r="AA112" s="72" t="s">
+      <c r="X112" s="79"/>
+      <c r="Y112" s="79"/>
+      <c r="AA112" s="78" t="s">
         <v>681</v>
       </c>
-      <c r="AB112" s="73"/>
-      <c r="AC112" s="73"/>
+      <c r="AB112" s="79"/>
+      <c r="AC112" s="79"/>
       <c r="AD112" s="71"/>
     </row>
-    <row r="113" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:30" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="45"/>
       <c r="B113" s="20" t="s">
         <v>570</v>
@@ -8252,7 +8249,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="114" spans="1:30" s="48" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:30" s="48" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114"/>
       <c r="B114" s="55" t="s">
         <v>589</v>
@@ -8307,7 +8304,7 @@
       <c r="AC114" s="9"/>
       <c r="AD114" s="9"/>
     </row>
-    <row r="115" spans="1:30" ht="60" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:30" ht="65" x14ac:dyDescent="0.2">
       <c r="B115" s="7" t="s">
         <v>650</v>
       </c>
@@ -8369,7 +8366,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="116" spans="1:30" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:30" ht="26" x14ac:dyDescent="0.2">
       <c r="E116" s="34"/>
       <c r="H116" s="13" t="s">
         <v>671</v>
@@ -8386,16 +8383,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O112:V112"/>
+    <mergeCell ref="W112:Y112"/>
+    <mergeCell ref="AA112:AC112"/>
+    <mergeCell ref="A93:A96"/>
+    <mergeCell ref="A85:A88"/>
     <mergeCell ref="L62:O62"/>
     <mergeCell ref="A5:A59"/>
     <mergeCell ref="B68:H68"/>
     <mergeCell ref="A62:A71"/>
     <mergeCell ref="A77:A82"/>
-    <mergeCell ref="O112:V112"/>
-    <mergeCell ref="W112:Y112"/>
-    <mergeCell ref="AA112:AC112"/>
-    <mergeCell ref="A93:A96"/>
-    <mergeCell ref="A85:A88"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <dataValidations count="9">
@@ -8433,2019 +8430,2019 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>450</v>
       </c>

</xml_diff>